<commit_message>
Added the new labeling updates.
</commit_message>
<xml_diff>
--- a/testing/Labeling/Data/Comments.xlsx
+++ b/testing/Labeling/Data/Comments.xlsx
@@ -5497,7 +5497,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="42.43"/>
+    <col customWidth="1" min="3" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>